<commit_message>
added results till 11
</commit_message>
<xml_diff>
--- a/Docs/StudyData/formal_algorithm/result.xlsx
+++ b/Docs/StudyData/formal_algorithm/result.xlsx
@@ -376,7 +376,7 @@
   <dimension ref="A1:I16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -646,20 +646,116 @@
       <c r="A11">
         <v>8</v>
       </c>
+      <c r="B11">
+        <v>99.2</v>
+      </c>
+      <c r="C11">
+        <v>97.6</v>
+      </c>
+      <c r="D11">
+        <v>97.6</v>
+      </c>
+      <c r="E11">
+        <v>97.540999999999997</v>
+      </c>
+      <c r="F11">
+        <v>100</v>
+      </c>
+      <c r="G11">
+        <v>98.4375</v>
+      </c>
+      <c r="H11">
+        <v>98.461500000000001</v>
+      </c>
+      <c r="I11">
+        <v>93.75</v>
+      </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>9</v>
       </c>
+      <c r="B12">
+        <v>93.700800000000001</v>
+      </c>
+      <c r="C12">
+        <v>91.406300000000002</v>
+      </c>
+      <c r="D12">
+        <v>98.412700000000001</v>
+      </c>
+      <c r="E12">
+        <v>98.4375</v>
+      </c>
+      <c r="F12">
+        <v>100</v>
+      </c>
+      <c r="G12">
+        <v>92.126000000000005</v>
+      </c>
+      <c r="H12">
+        <v>99.180300000000003</v>
+      </c>
+      <c r="I12">
+        <v>99.212599999999995</v>
+      </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>10</v>
       </c>
+      <c r="B13">
+        <v>94.262299999999996</v>
+      </c>
+      <c r="C13">
+        <v>89.843800000000002</v>
+      </c>
+      <c r="D13">
+        <v>89.344300000000004</v>
+      </c>
+      <c r="E13">
+        <v>89.843800000000002</v>
+      </c>
+      <c r="F13">
+        <v>98.333299999999994</v>
+      </c>
+      <c r="G13">
+        <v>98.425200000000004</v>
+      </c>
+      <c r="H13">
+        <v>94.166700000000006</v>
+      </c>
+      <c r="I13">
+        <v>97.637799999999999</v>
+      </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>11</v>
+      </c>
+      <c r="B14">
+        <v>95.2</v>
+      </c>
+      <c r="C14">
+        <v>98.319299999999998</v>
+      </c>
+      <c r="D14">
+        <v>91.2</v>
+      </c>
+      <c r="E14">
+        <v>94.117599999999996</v>
+      </c>
+      <c r="F14">
+        <v>99.206299999999999</v>
+      </c>
+      <c r="G14">
+        <v>100</v>
+      </c>
+      <c r="H14">
+        <v>96.031700000000001</v>
+      </c>
+      <c r="I14">
+        <v>100</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
updated to version 0.5.5
</commit_message>
<xml_diff>
--- a/Docs/StudyData/formal_algorithm/result.xlsx
+++ b/Docs/StudyData/formal_algorithm/result.xlsx
@@ -9,12 +9,12 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="12">
   <si>
     <t>fingertip</t>
   </si>
@@ -32,6 +32,24 @@
   </si>
   <si>
     <t>horizontal</t>
+  </si>
+  <si>
+    <t>delete the biggest and smallest</t>
+  </si>
+  <si>
+    <t>average</t>
+  </si>
+  <si>
+    <t>without nail</t>
+  </si>
+  <si>
+    <t>with nail</t>
+  </si>
+  <si>
+    <t>on finger</t>
+  </si>
+  <si>
+    <t>on wrist</t>
   </si>
 </sst>
 </file>
@@ -84,6 +102,1217 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="zh-CN"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$47</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>on finger</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-1.9469660690808513E-17"/>
+                  <c:y val="0.22789371553274942"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="outEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-3.8939321381617026E-17"/>
+                  <c:y val="0.24986746881358932"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="outEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-7.7878642763234052E-17"/>
+                  <c:y val="0.27634008670264532"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="outEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="3"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0"/>
+                  <c:y val="0.33190114718806213"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="outEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="3200" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="ctr"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:errBars>
+            <c:errBarType val="both"/>
+            <c:errValType val="stdErr"/>
+            <c:noEndCap val="0"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="dk1"/>
+                </a:solidFill>
+                <a:prstDash val="solid"/>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>Sheet1!$B$45:$E$46</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="4"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>without nail</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>with nail</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>without nail</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>with nail</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>vertical</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>horizontal</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$47:$E$47</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>95.826580000000007</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>91.94165000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>99.503960000000006</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>97.952069999999992</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$48</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>on wrist</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="3"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-1.557572855264681E-16"/>
+                  <c:y val="0.29499165413312101"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="outEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="3200" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="ctr"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:errBars>
+            <c:errBarType val="both"/>
+            <c:errValType val="stdErr"/>
+            <c:noEndCap val="0"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="dk1"/>
+                </a:solidFill>
+                <a:prstDash val="solid"/>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>Sheet1!$B$45:$E$46</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="4"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>without nail</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>with nail</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>without nail</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>with nail</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>vertical</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>horizontal</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$48:$E$48</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>93.76885</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>94.047789999999992</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>96.785850000000011</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>98.926399999999987</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="ctr"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="1821595840"/>
+        <c:axId val="1821596384"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1821595840"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="bg1">
+                <a:lumMod val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:prstDash val="solid"/>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="4000" b="1" i="0" u="none" strike="noStrike" kern="100" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1821596384"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1821596384"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="102"/>
+          <c:min val="80"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="bg1">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:prstDash val="solid"/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="4000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1821595840"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+        <c:majorUnit val="5"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="7.0091588181564815E-2"/>
+          <c:y val="3.0948007903506443E-2"/>
+          <c:w val="0.54099141214982738"/>
+          <c:h val="6.6927836267657553E-2"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="4000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="bg1">
+          <a:lumMod val="75000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>280986</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="9" name="图表 8"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -373,10 +1602,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I16"/>
+  <dimension ref="A1:I55"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -762,13 +1991,474 @@
       <c r="A15">
         <v>12</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>13</v>
+      <c r="B15">
+        <v>94.354799999999997</v>
+      </c>
+      <c r="C15">
+        <v>80.3279</v>
+      </c>
+      <c r="D15">
+        <v>89.516099999999994</v>
+      </c>
+      <c r="E15">
+        <v>92.623000000000005</v>
+      </c>
+      <c r="F15">
+        <v>90.598299999999995</v>
+      </c>
+      <c r="G15">
+        <v>98.360699999999994</v>
+      </c>
+      <c r="H15">
+        <v>83.7607</v>
+      </c>
+      <c r="I15">
+        <v>99.180300000000003</v>
+      </c>
+    </row>
+    <row r="28" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="29" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
+        <v>4</v>
+      </c>
+      <c r="F29" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="32" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B32">
+        <v>93.700800000000001</v>
+      </c>
+      <c r="C32">
+        <v>83.593800000000002</v>
+      </c>
+      <c r="D32">
+        <v>88.181799999999996</v>
+      </c>
+      <c r="E32">
+        <v>86.087000000000003</v>
+      </c>
+      <c r="F32">
+        <v>98.333299999999994</v>
+      </c>
+      <c r="G32">
+        <v>95.041300000000007</v>
+      </c>
+      <c r="H32">
+        <v>92.5</v>
+      </c>
+      <c r="I32">
+        <v>97.5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B33">
+        <v>93.75</v>
+      </c>
+      <c r="C33">
+        <v>86.956500000000005</v>
+      </c>
+      <c r="D33">
+        <v>89.344300000000004</v>
+      </c>
+      <c r="E33">
+        <v>89.843800000000002</v>
+      </c>
+      <c r="F33">
+        <v>98.333299999999994</v>
+      </c>
+      <c r="G33">
+        <v>96.666700000000006</v>
+      </c>
+      <c r="H33">
+        <v>94.166700000000006</v>
+      </c>
+      <c r="I33">
+        <v>97.637799999999999</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B34">
+        <v>94.262299999999996</v>
+      </c>
+      <c r="C34">
+        <v>88.372100000000003</v>
+      </c>
+      <c r="D34">
+        <v>89.516099999999994</v>
+      </c>
+      <c r="E34">
+        <v>91.869900000000001</v>
+      </c>
+      <c r="F34">
+        <v>99.166700000000006</v>
+      </c>
+      <c r="G34">
+        <v>97.6</v>
+      </c>
+      <c r="H34">
+        <v>95.614000000000004</v>
+      </c>
+      <c r="I34">
+        <v>98.333299999999994</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B35">
+        <v>94.354799999999997</v>
+      </c>
+      <c r="C35">
+        <v>89.843800000000002</v>
+      </c>
+      <c r="D35">
+        <v>91.2</v>
+      </c>
+      <c r="E35">
+        <v>92.623000000000005</v>
+      </c>
+      <c r="F35">
+        <v>99.206299999999999</v>
+      </c>
+      <c r="G35">
+        <v>97.656300000000002</v>
+      </c>
+      <c r="H35">
+        <v>96.031700000000001</v>
+      </c>
+      <c r="I35">
+        <v>98.4</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B36">
+        <v>94.495400000000004</v>
+      </c>
+      <c r="C36">
+        <v>91.406300000000002</v>
+      </c>
+      <c r="D36">
+        <v>95.3125</v>
+      </c>
+      <c r="E36">
+        <v>93.846199999999996</v>
+      </c>
+      <c r="F36">
+        <v>100</v>
+      </c>
+      <c r="G36">
+        <v>98.332999999999998</v>
+      </c>
+      <c r="H36">
+        <v>96.748000000000005</v>
+      </c>
+      <c r="I36">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B37">
+        <v>95.2</v>
+      </c>
+      <c r="C37">
+        <v>92.307699999999997</v>
+      </c>
+      <c r="D37">
+        <v>95.412800000000004</v>
+      </c>
+      <c r="E37">
+        <v>94.117599999999996</v>
+      </c>
+      <c r="F37">
+        <v>100</v>
+      </c>
+      <c r="G37">
+        <v>98.360699999999994</v>
+      </c>
+      <c r="H37">
+        <v>97.5</v>
+      </c>
+      <c r="I37">
+        <v>99.180300000000003</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B38">
+        <v>96.031700000000001</v>
+      </c>
+      <c r="C38">
+        <v>95.081999999999994</v>
+      </c>
+      <c r="D38">
+        <v>95.833299999999994</v>
+      </c>
+      <c r="E38">
+        <v>97.540999999999997</v>
+      </c>
+      <c r="F38">
+        <v>100</v>
+      </c>
+      <c r="G38">
+        <v>98.425200000000004</v>
+      </c>
+      <c r="H38">
+        <v>98.4375</v>
+      </c>
+      <c r="I38">
+        <v>99.212599999999995</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B39">
+        <v>98.4375</v>
+      </c>
+      <c r="C39">
+        <v>95.935000000000002</v>
+      </c>
+      <c r="D39">
+        <v>96.875</v>
+      </c>
+      <c r="E39">
+        <v>97.674400000000006</v>
+      </c>
+      <c r="F39">
+        <v>100</v>
+      </c>
+      <c r="G39">
+        <v>98.4375</v>
+      </c>
+      <c r="H39">
+        <v>98.461500000000001</v>
+      </c>
+      <c r="I39">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B40">
+        <v>98.833299999999994</v>
+      </c>
+      <c r="C40">
+        <v>97.6</v>
+      </c>
+      <c r="D40">
+        <v>97.6</v>
+      </c>
+      <c r="E40">
+        <v>98.4375</v>
+      </c>
+      <c r="F40">
+        <v>100</v>
+      </c>
+      <c r="G40">
+        <v>99</v>
+      </c>
+      <c r="H40">
+        <v>99.180300000000003</v>
+      </c>
+      <c r="I40">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B41">
+        <v>99.2</v>
+      </c>
+      <c r="C41">
+        <v>98.319299999999998</v>
+      </c>
+      <c r="D41">
+        <v>98.412700000000001</v>
+      </c>
+      <c r="E41">
+        <v>98.4375</v>
+      </c>
+      <c r="F41">
+        <v>100</v>
+      </c>
+      <c r="G41">
+        <v>100</v>
+      </c>
+      <c r="H41">
+        <v>99.218800000000002</v>
+      </c>
+      <c r="I41">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>7</v>
+      </c>
+      <c r="B43">
+        <f>AVERAGE(B32:B41)</f>
+        <v>95.826580000000007</v>
+      </c>
+      <c r="C43">
+        <f t="shared" ref="C43:I43" si="0">AVERAGE(C32:C41)</f>
+        <v>91.94165000000001</v>
+      </c>
+      <c r="D43">
+        <f t="shared" si="0"/>
+        <v>93.76885</v>
+      </c>
+      <c r="E43">
+        <f t="shared" si="0"/>
+        <v>94.047789999999992</v>
+      </c>
+      <c r="F43">
+        <f t="shared" si="0"/>
+        <v>99.503960000000006</v>
+      </c>
+      <c r="G43">
+        <f t="shared" si="0"/>
+        <v>97.952069999999992</v>
+      </c>
+      <c r="H43">
+        <f t="shared" si="0"/>
+        <v>96.785850000000011</v>
+      </c>
+      <c r="I43">
+        <f t="shared" si="0"/>
+        <v>98.926399999999987</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B45" t="s">
+        <v>4</v>
+      </c>
+      <c r="D45" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B46" t="s">
+        <v>8</v>
+      </c>
+      <c r="C46" t="s">
+        <v>9</v>
+      </c>
+      <c r="D46" t="s">
+        <v>8</v>
+      </c>
+      <c r="E46" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>10</v>
+      </c>
+      <c r="B47">
+        <f>B43</f>
+        <v>95.826580000000007</v>
+      </c>
+      <c r="C47">
+        <f>C43</f>
+        <v>91.94165000000001</v>
+      </c>
+      <c r="D47">
+        <f>F43</f>
+        <v>99.503960000000006</v>
+      </c>
+      <c r="E47">
+        <f>G43</f>
+        <v>97.952069999999992</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>11</v>
+      </c>
+      <c r="B48">
+        <f>D43</f>
+        <v>93.76885</v>
+      </c>
+      <c r="C48">
+        <f>E43</f>
+        <v>94.047789999999992</v>
+      </c>
+      <c r="D48">
+        <f>H43</f>
+        <v>96.785850000000011</v>
+      </c>
+      <c r="E48">
+        <f>I43</f>
+        <v>98.926399999999987</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B52" t="s">
+        <v>4</v>
+      </c>
+      <c r="D52" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B53" t="s">
+        <v>10</v>
+      </c>
+      <c r="C53" t="s">
+        <v>11</v>
+      </c>
+      <c r="D53" t="s">
+        <v>10</v>
+      </c>
+      <c r="E53" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>8</v>
+      </c>
+      <c r="B54">
+        <f>B43</f>
+        <v>95.826580000000007</v>
+      </c>
+      <c r="C54">
+        <f>D43</f>
+        <v>93.76885</v>
+      </c>
+      <c r="D54">
+        <f>F43</f>
+        <v>99.503960000000006</v>
+      </c>
+      <c r="E54">
+        <f>H43</f>
+        <v>96.785850000000011</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>9</v>
+      </c>
+      <c r="B55">
+        <f>C43</f>
+        <v>91.94165000000001</v>
+      </c>
+      <c r="C55">
+        <f>E43</f>
+        <v>94.047789999999992</v>
+      </c>
+      <c r="D55">
+        <f>G43</f>
+        <v>97.952069999999992</v>
+      </c>
+      <c r="E55">
+        <f>I43</f>
+        <v>98.926399999999987</v>
       </c>
     </row>
   </sheetData>
+  <sortState ref="D28:D39">
+    <sortCondition ref="D28:D39"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>